<commit_message>
change table's header name
</commit_message>
<xml_diff>
--- a/BackEnd/public/table2.xlsx
+++ b/BackEnd/public/table2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i_rin/Desktop/tablevis/BackEnd/public/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\tablevis\BackEnd\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85B31EE-68FA-A24E-A439-58B578150AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56E9C23-9E0F-4862-8EEC-8921C0168E04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{2EFAC2C9-10E9-47BE-B617-40AF9808DAEE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="30">
   <si>
     <t>2013</t>
   </si>
@@ -115,12 +115,16 @@
     <t>0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Sony</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,6 +267,18 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -272,13 +288,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -287,17 +297,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -615,73 +619,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9D183D6-0C77-44FB-8CFA-EC3E3E690E7B}">
   <dimension ref="A1:AI42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
-      <c r="A1" s="11"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9" t="s">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A1" s="15"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9" t="s">
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9" t="s">
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9" t="s">
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9" t="s">
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
-      <c r="AA1" s="9"/>
-      <c r="AB1" s="9" t="s">
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="AC1" s="9"/>
-      <c r="AD1" s="9"/>
-      <c r="AE1" s="9"/>
-      <c r="AF1" s="9" t="s">
+      <c r="AC1" s="13"/>
+      <c r="AD1" s="13"/>
+      <c r="AE1" s="13"/>
+      <c r="AF1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="AG1" s="9"/>
-      <c r="AH1" s="9"/>
-      <c r="AI1" s="10"/>
+      <c r="AG1" s="13"/>
+      <c r="AH1" s="13"/>
+      <c r="AI1" s="14"/>
     </row>
-    <row r="2" spans="1:35" ht="16" thickBot="1">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="19"/>
+    <row r="2" spans="1:35" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="20"/>
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
@@ -779,11 +783,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:35">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -886,9 +890,9 @@
         <v>9.9999999999980105</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
-      <c r="A4" s="12"/>
-      <c r="B4" s="14"/>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="3" t="s">
         <v>26</v>
       </c>
@@ -989,9 +993,9 @@
         <v>19.999999999999574</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
-      <c r="A5" s="12"/>
-      <c r="B5" s="14"/>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1092,9 +1096,9 @@
         <v>70.000000000000284</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
-      <c r="A6" s="12"/>
-      <c r="B6" s="14"/>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="3" t="s">
         <v>27</v>
       </c>
@@ -1195,9 +1199,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35">
-      <c r="A7" s="12"/>
-      <c r="B7" s="14" t="s">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1300,9 +1304,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:35">
-      <c r="A8" s="12"/>
-      <c r="B8" s="14"/>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="3" t="s">
         <v>26</v>
       </c>
@@ -1403,9 +1407,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
-      <c r="A9" s="12"/>
-      <c r="B9" s="14"/>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="3" t="s">
         <v>15</v>
       </c>
@@ -1506,9 +1510,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
-      <c r="A10" s="12"/>
-      <c r="B10" s="14"/>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="3" t="s">
         <v>27</v>
       </c>
@@ -1609,9 +1613,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:35">
-      <c r="A11" s="12"/>
-      <c r="B11" s="14" t="s">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -1714,9 +1718,9 @@
         <v>1740.000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:35">
-      <c r="A12" s="12"/>
-      <c r="B12" s="14"/>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="3" t="s">
         <v>26</v>
       </c>
@@ -1817,9 +1821,9 @@
         <v>1259.9999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:35">
-      <c r="A13" s="12"/>
-      <c r="B13" s="14"/>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="3" t="s">
         <v>15</v>
       </c>
@@ -1920,9 +1924,9 @@
         <v>2549.9999999999973</v>
       </c>
     </row>
-    <row r="14" spans="1:35">
-      <c r="A14" s="12"/>
-      <c r="B14" s="14"/>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="3" t="s">
         <v>27</v>
       </c>
@@ -2023,9 +2027,9 @@
         <v>900.00000000000034</v>
       </c>
     </row>
-    <row r="15" spans="1:35">
-      <c r="A15" s="12"/>
-      <c r="B15" s="14" t="s">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -2128,9 +2132,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:35">
-      <c r="A16" s="12"/>
-      <c r="B16" s="14"/>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="3" t="s">
         <v>26</v>
       </c>
@@ -2231,9 +2235,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:35">
-      <c r="A17" s="12"/>
-      <c r="B17" s="14"/>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="3" t="s">
         <v>15</v>
       </c>
@@ -2334,9 +2338,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:35">
-      <c r="A18" s="12"/>
-      <c r="B18" s="14"/>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="3" t="s">
         <v>27</v>
       </c>
@@ -2437,9 +2441,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:35">
-      <c r="A19" s="12"/>
-      <c r="B19" s="14" t="s">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -2542,9 +2546,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:35">
-      <c r="A20" s="12"/>
-      <c r="B20" s="14"/>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="3" t="s">
         <v>26</v>
       </c>
@@ -2645,9 +2649,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:35">
-      <c r="A21" s="12"/>
-      <c r="B21" s="14"/>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="3" t="s">
         <v>15</v>
       </c>
@@ -2748,9 +2752,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:35">
-      <c r="A22" s="12"/>
-      <c r="B22" s="14"/>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="3" t="s">
         <v>27</v>
       </c>
@@ -2851,9 +2855,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:35">
-      <c r="A23" s="12"/>
-      <c r="B23" s="14" t="s">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -2956,9 +2962,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:35">
-      <c r="A24" s="12"/>
-      <c r="B24" s="14"/>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="3" t="s">
         <v>26</v>
       </c>
@@ -3059,9 +3065,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:35">
-      <c r="A25" s="12"/>
-      <c r="B25" s="14"/>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="3" t="s">
         <v>15</v>
       </c>
@@ -3162,9 +3168,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:35">
-      <c r="A26" s="12"/>
-      <c r="B26" s="14"/>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="3" t="s">
         <v>27</v>
       </c>
@@ -3265,9 +3271,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:35">
-      <c r="A27" s="12"/>
-      <c r="B27" s="14" t="s">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A27" s="9"/>
+      <c r="B27" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -3370,9 +3376,9 @@
         <v>560.00000000000227</v>
       </c>
     </row>
-    <row r="28" spans="1:35">
-      <c r="A28" s="12"/>
-      <c r="B28" s="14"/>
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="3" t="s">
         <v>26</v>
       </c>
@@ -3473,9 +3479,9 @@
         <v>39.999999999999147</v>
       </c>
     </row>
-    <row r="29" spans="1:35">
-      <c r="A29" s="12"/>
-      <c r="B29" s="14"/>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A29" s="9"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="3" t="s">
         <v>15</v>
       </c>
@@ -3576,9 +3582,9 @@
         <v>419.9999999999946</v>
       </c>
     </row>
-    <row r="30" spans="1:35">
-      <c r="A30" s="12"/>
-      <c r="B30" s="14"/>
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A30" s="9"/>
+      <c r="B30" s="11"/>
       <c r="C30" s="3" t="s">
         <v>27</v>
       </c>
@@ -3679,9 +3685,9 @@
         <v>109.99999999999943</v>
       </c>
     </row>
-    <row r="31" spans="1:35">
-      <c r="A31" s="12"/>
-      <c r="B31" s="14" t="s">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A31" s="9"/>
+      <c r="B31" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -3784,9 +3790,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:35">
-      <c r="A32" s="12"/>
-      <c r="B32" s="14"/>
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A32" s="9"/>
+      <c r="B32" s="11"/>
       <c r="C32" s="3" t="s">
         <v>26</v>
       </c>
@@ -3887,9 +3893,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:35">
-      <c r="A33" s="12"/>
-      <c r="B33" s="14"/>
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A33" s="9"/>
+      <c r="B33" s="11"/>
       <c r="C33" s="3" t="s">
         <v>15</v>
       </c>
@@ -3990,9 +3996,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:35">
-      <c r="A34" s="12"/>
-      <c r="B34" s="14"/>
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A34" s="9"/>
+      <c r="B34" s="11"/>
       <c r="C34" s="3" t="s">
         <v>27</v>
       </c>
@@ -4093,11 +4099,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:35">
-      <c r="A35" s="12" t="s">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C35" s="3" t="s">
@@ -4200,9 +4206,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:35">
-      <c r="A36" s="12"/>
-      <c r="B36" s="14"/>
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A36" s="9"/>
+      <c r="B36" s="11"/>
       <c r="C36" s="3" t="s">
         <v>26</v>
       </c>
@@ -4303,9 +4309,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:35">
-      <c r="A37" s="12"/>
-      <c r="B37" s="14"/>
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A37" s="9"/>
+      <c r="B37" s="11"/>
       <c r="C37" s="3" t="s">
         <v>15</v>
       </c>
@@ -4406,9 +4412,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:35">
-      <c r="A38" s="12"/>
-      <c r="B38" s="14"/>
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A38" s="9"/>
+      <c r="B38" s="11"/>
       <c r="C38" s="3" t="s">
         <v>27</v>
       </c>
@@ -4509,9 +4515,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:35">
-      <c r="A39" s="12"/>
-      <c r="B39" s="14" t="s">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A39" s="9"/>
+      <c r="B39" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -4614,9 +4620,9 @@
         <v>70.000000000000284</v>
       </c>
     </row>
-    <row r="40" spans="1:35">
-      <c r="A40" s="12"/>
-      <c r="B40" s="14"/>
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A40" s="9"/>
+      <c r="B40" s="11"/>
       <c r="C40" s="3" t="s">
         <v>26</v>
       </c>
@@ -4717,9 +4723,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:35">
-      <c r="A41" s="12"/>
-      <c r="B41" s="14"/>
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A41" s="9"/>
+      <c r="B41" s="11"/>
       <c r="C41" s="3" t="s">
         <v>15</v>
       </c>
@@ -4820,9 +4826,9 @@
         <v>149.99999999999858</v>
       </c>
     </row>
-    <row r="42" spans="1:35" ht="16" thickBot="1">
-      <c r="A42" s="17"/>
-      <c r="B42" s="20"/>
+    <row r="42" spans="1:35" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="10"/>
+      <c r="B42" s="12"/>
       <c r="C42" s="4" t="s">
         <v>27</v>
       </c>
@@ -4925,13 +4931,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="A23:A34"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="B31:B34"/>
     <mergeCell ref="X1:AA1"/>
     <mergeCell ref="AB1:AE1"/>
     <mergeCell ref="AF1:AI1"/>
@@ -4947,6 +4946,13 @@
     <mergeCell ref="L1:O1"/>
     <mergeCell ref="P1:S1"/>
     <mergeCell ref="T1:W1"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="A23:A34"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="B31:B34"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>